<commit_message>
Made further changes to model
</commit_message>
<xml_diff>
--- a/model-design/solver-implementation.xlsx
+++ b/model-design/solver-implementation.xlsx
@@ -8,8 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet1!$C$15:$D$17</definedName>
@@ -20,14 +19,17 @@
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">Sheet1!$C$15:$D$17</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">Sheet1!$C$28</definedName>
-    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Sheet1!$E$22:$E$24</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Sheet1!$C$32</definedName>
+    <definedName name="solver_lhs4" localSheetId="0" hidden="1">Sheet1!$C$33</definedName>
+    <definedName name="solver_lhs5" localSheetId="0" hidden="1">Sheet1!$E$22:$E$24</definedName>
+    <definedName name="solver_lhs6" localSheetId="0" hidden="1">Sheet1!$E$22:$E$24</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">5</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$E$4</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
@@ -35,9 +37,15 @@
     <definedName name="solver_rel1" localSheetId="0" hidden="1">4</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel4" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel5" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel6" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">integer</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">Sheet1!$D$28</definedName>
-    <definedName name="solver_rhs3" localSheetId="0" hidden="1">Sheet1!$G$22:$G$24</definedName>
+    <definedName name="solver_rhs3" localSheetId="0" hidden="1">Sheet1!$D$32</definedName>
+    <definedName name="solver_rhs4" localSheetId="0" hidden="1">Sheet1!$D$33</definedName>
+    <definedName name="solver_rhs5" localSheetId="0" hidden="1">Sheet1!$G$22:$G$24</definedName>
+    <definedName name="solver_rhs6" localSheetId="0" hidden="1">Sheet1!$G$22:$G$24</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
@@ -54,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
     <t>Bags</t>
   </si>
@@ -117,6 +125,42 @@
   </si>
   <si>
     <t>Capacity</t>
+  </si>
+  <si>
+    <t>Area 1</t>
+  </si>
+  <si>
+    <t>LPC</t>
+  </si>
+  <si>
+    <t>Small</t>
+  </si>
+  <si>
+    <t>Nano</t>
+  </si>
+  <si>
+    <t>Finishing Capacity</t>
+  </si>
+  <si>
+    <t>Container Type</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>Stations</t>
+  </si>
+  <si>
+    <t>Total Rate</t>
+  </si>
+  <si>
+    <t>MPC/MPCL</t>
+  </si>
+  <si>
+    <t>Bagging @ 120 uph; 2 upp</t>
+  </si>
+  <si>
+    <t>Man. Pack @ 60 uph;  2upp</t>
   </si>
 </sst>
 </file>
@@ -216,7 +260,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -239,14 +283,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -549,30 +598,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G28"/>
+  <dimension ref="B1:G43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37:E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
@@ -584,10 +633,10 @@
       <c r="E3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="16" t="s">
         <v>19</v>
       </c>
     </row>
@@ -597,15 +646,15 @@
       </c>
       <c r="C4" s="3">
         <f>SUM(C22:C24)</f>
-        <v>854</v>
+        <v>720</v>
       </c>
       <c r="D4" s="3">
         <f>SUM(D22:D24)</f>
-        <v>3416</v>
+        <v>1080</v>
       </c>
       <c r="E4" s="4">
         <f>SUM(C4:D4)</f>
-        <v>4270</v>
+        <v>1800</v>
       </c>
       <c r="F4" s="2">
         <f>SUM(G22:G24)</f>
@@ -613,7 +662,7 @@
       </c>
       <c r="G4" s="19">
         <f>E4/F4</f>
-        <v>0.83235867446393763</v>
+        <v>0.35087719298245612</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
@@ -688,7 +737,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="5">
-        <v>850</v>
+        <v>720</v>
       </c>
       <c r="D15" s="5">
         <v>0</v>
@@ -703,7 +752,7 @@
         <v>0</v>
       </c>
       <c r="D16" s="5">
-        <v>1710</v>
+        <v>540</v>
       </c>
       <c r="E16" s="8"/>
     </row>
@@ -712,10 +761,10 @@
         <v>3</v>
       </c>
       <c r="C17" s="5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D17" s="5">
-        <v>1706</v>
+        <v>540</v>
       </c>
       <c r="E17" s="8"/>
     </row>
@@ -753,7 +802,7 @@
       </c>
       <c r="C22" s="5">
         <f>C15 *C10</f>
-        <v>850</v>
+        <v>720</v>
       </c>
       <c r="D22" s="5">
         <f>D15*D10</f>
@@ -761,7 +810,7 @@
       </c>
       <c r="E22" s="10">
         <f>SUM(C22:D22)</f>
-        <v>850</v>
+        <v>720</v>
       </c>
       <c r="F22" s="9" t="s">
         <v>6</v>
@@ -780,11 +829,11 @@
       </c>
       <c r="D23" s="5">
         <f t="shared" ref="D23:D24" si="0">D16*D11</f>
-        <v>1710</v>
+        <v>540</v>
       </c>
       <c r="E23" s="10">
         <f t="shared" ref="E23:E24" si="1">SUM(C23:D23)</f>
-        <v>1710</v>
+        <v>540</v>
       </c>
       <c r="F23" s="9" t="s">
         <v>6</v>
@@ -799,15 +848,15 @@
       </c>
       <c r="C24" s="5">
         <f>C17 *C12</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D24" s="5">
         <f t="shared" si="0"/>
-        <v>1706</v>
+        <v>540</v>
       </c>
       <c r="E24" s="10">
         <f t="shared" si="1"/>
-        <v>1710</v>
+        <v>540</v>
       </c>
       <c r="F24" s="9" t="s">
         <v>6</v>
@@ -822,15 +871,15 @@
       </c>
       <c r="C25" s="12">
         <f>SUM(C22:C24)</f>
-        <v>854</v>
+        <v>720</v>
       </c>
       <c r="D25" s="12">
         <f t="shared" ref="D25:E25" si="2">SUM(D22:D24)</f>
-        <v>3416</v>
+        <v>1080</v>
       </c>
       <c r="E25" s="13">
         <f t="shared" si="2"/>
-        <v>4270</v>
+        <v>1800</v>
       </c>
       <c r="F25" s="14" t="s">
         <v>6</v>
@@ -861,19 +910,169 @@
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="C28" s="2">
         <f>SUM(C22:C24)</f>
-        <v>854</v>
+        <v>720</v>
       </c>
       <c r="D28" s="2">
         <f xml:space="preserve"> B28 * SUM(C22:D24)</f>
-        <v>854</v>
+        <v>720</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="20">
+        <f>D25</f>
+        <v>1080</v>
+      </c>
+      <c r="D32" s="20">
+        <v>4140</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="20">
+        <f>C25</f>
+        <v>720</v>
+      </c>
+      <c r="D33" s="20">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="E36" s="24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37" s="23">
+        <v>720</v>
+      </c>
+      <c r="D37" s="23">
+        <v>1</v>
+      </c>
+      <c r="E37" s="23">
+        <f>C37 * D37</f>
+        <v>720</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" s="23">
+        <v>810</v>
+      </c>
+      <c r="D38" s="23">
+        <v>2</v>
+      </c>
+      <c r="E38" s="23">
+        <f t="shared" ref="E38:E42" si="3">C38 * D38</f>
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" s="23">
+        <v>840</v>
+      </c>
+      <c r="D39" s="23">
+        <v>1</v>
+      </c>
+      <c r="E39" s="23">
+        <f t="shared" si="3"/>
+        <v>840</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C40" s="23">
+        <v>960</v>
+      </c>
+      <c r="D40" s="23">
+        <v>1</v>
+      </c>
+      <c r="E40" s="23">
+        <f t="shared" si="3"/>
+        <v>960</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41" s="22">
+        <v>60</v>
+      </c>
+      <c r="D41" s="22">
+        <v>12</v>
+      </c>
+      <c r="E41" s="22">
+        <f t="shared" si="3"/>
+        <v>720</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C42" s="22">
+        <v>30</v>
+      </c>
+      <c r="D42" s="22">
+        <v>60</v>
+      </c>
+      <c r="E42" s="22">
+        <f t="shared" si="3"/>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" s="23"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="23">
+        <f>SUM(E37:E42)</f>
+        <v>6660</v>
       </c>
     </row>
   </sheetData>
-  <scenarios current="0" show="0" sqref="L4">
+  <scenarios current="1" show="0" sqref="L4">
     <scenario name="Bags @ 42%" count="6" user="Isaac Adjei-Attah" comment="Created by Isaac Adjei-Attah on 4/28/2019">
       <inputCells r="C15" val="1688"/>
       <inputCells r="D15" val="0"/>
@@ -882,6 +1081,14 @@
       <inputCells r="C17" val="454"/>
       <inputCells r="D17" val="1255"/>
     </scenario>
+    <scenario name="Bags @40%" count="6" user="Isaac Adjei-Attah" comment="Created by Isaac Adjei-Attah on 4/28/2019">
+      <inputCells r="C15" val="720"/>
+      <inputCells r="D15" val="0"/>
+      <inputCells r="C16" val="0"/>
+      <inputCells r="D16" val="337"/>
+      <inputCells r="C17" val="0"/>
+      <inputCells r="D17" val="743"/>
+    </scenario>
   </scenarios>
   <mergeCells count="3">
     <mergeCell ref="B1:G1"/>
@@ -889,6 +1096,7 @@
     <mergeCell ref="B19:E19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -902,16 +1110,4 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>